<commit_message>
Added a few fixes to the techniques table
</commit_message>
<xml_diff>
--- a/scripts/matrix.xlsx
+++ b/scripts/matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/svitlana/Documents/projects/threat-matrix-CN/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4A4729-9B52-154F-9077-1FE2641CF5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A83701-DA1B-0E48-BECF-8F647F89BEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CNMatrixMapping_sh" sheetId="1" r:id="rId1"/>
@@ -31,2159 +31,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Microsoft Office User</author>
-  </authors>
-  <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{78DBDF49-6DD4-7645-8D92-2FBA19BDABFD}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-0.0.01.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">may use compromised credentials of existing accounts. Obtained certificates may give increased privileges and provide access to restricted network areas. Not using malware can make detecting the presence of an adversary harder. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Source: https://attack.mitre.org/techniques/T1078/</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{ADA66C82-BA17-324A-9B74-CCB5B4BCB431}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-1.0.01.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may publish a malicious image in the public repository. Adversaries may try to hide the fact that the image is malicious by matching a legitimate name. Thus users might use the image without realizing that it is malicious. This leads to the execution of code that can be used for starting cryptocurrency mining in the instance or container. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Source: https://attack.mitre.org/techniques/T1204/003/</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{7C57FB9F-C5CC-0141-A214-23D5DFED3DAE}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-3.0.01.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may use compromised credentials of existing accounts. Obtained certificates may give increased privileges and provide access to restricted network areas. Not using malware can make detecting the presence of an adversary harder. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Source: https://attack.mitre.org/techniques/T1078/
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{5782BD8D-7AC9-254B-B63A-CB94BFEA3902}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-4.0.01.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may use compromised credentials of existing accounts. Obtained certificates may give increased privileges and provide access to restricted network areas. Not using malware can make detecting the presence of an adversary harder. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Source: https://attack.mitre.org/techniques/T1078/
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{84952447-D451-2C49-B54C-AB0EBCF67EDC}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-5.0.01.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may use compromised credentials of existing accounts. Obtained certificates may give increased privileges and provide access to restricted network areas. Not using malware can make detecting the presence of an adversary harder. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Source: https://attack.mitre.org/techniques/T1078/
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{F30D241D-601E-3A43-85A1-4D1A5441AE9E}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-0.0.02.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">may access the system via external remote services (e.g., VPNs), which allows them to connect from the remote location to the system. In the case of containerized environments, there are sensitive interfaces that are not meant to be exposed publicly. But sometimes due to misconfigured environments, they can be exposed. As they don't require authentication adversaries can use them to deploy a container or run malicious code. Examples of those interfaces are Docker API, Kubernetes API server, kublet, Kubeflow. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Source: https://attack.mitre.org/techniques/T1133/ https://www.microsoft.com/security/blog/2021/03/23/secure-containerized-environments-with-updated-threat-matrix-for-kubernetes/</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{AFA94B5D-E7E1-914A-908F-922A83EC7688}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-1.2.02. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may compromise the container administration services such as kublet, the Kubernetes API server, and the Docker daemon. This can allow them to remotely manage containers in the environment and execute commands. For example, in Docker, the docker exec can be used to execute commands in the running container. In the Kubernetes, execution of commands can be gained by using kubectl exec, the kublet, the Kubernetes API server, and having a proper access level.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Source: https://attack.mitre.org/techniques/T1609/ </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{B0BFFA45-1D37-E64C-AF02-BD6FCF55BF76}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-3.0.02.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may implant or backdoor a malicious cloud or container image. For example, the adversary can embed docker images, Google Cloud Platform images, Amazon Machine Images, and Azure images in the user's environment after gaining initial access.  Having access to a compromised cloud environment and listing available images allows an adversary to implant a backdoor in the container images. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Source: https://attack.mitre.org/techniques/T1525/</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{A06B6773-E7A4-1945-B41F-451D5E3DD88F}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-4.2.02.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may escape from the container to the host environment, which gives them an access to other containers and/or the underlying host. The main cause of this is typically containerized environments that don't have a separation from the host environment. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Source: https://attack.mitre.org/techniques/T1611/  </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{15DA2354-8A46-E442-BDE8-B29FAD3212BB}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-5.0.02.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may turn off, exhaust, or block the defensive mechanisms of a target system. Defensive mechanisms include firewalls, audit logs, and security tools. Having these mechanisms disabled allows adversaries to avoid detecting malicious activities and system modification. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">In cloud environments, modifying cloud firewall rules allow bypassing limitations on accessing cloud resources. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Source: https://attack.mitre.org/techniques/T1562/  https://attack.mitre.org/techniques/T1562/007/ </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{E2E81CB6-3A24-744D-93A2-D92FFC1D74CF}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-0.0.03. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may exploit the weakest/less secure link in the CI/CD pipeline. Mainly targeted areas are exploits on widely used open-source packages, open-source vulnerabilities, compromised CI/CD tools, and changes in the build process.  
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">In 2021 suply chain attacks increased by 300% compared to 2020 based on the Aqua "2021 Software Supply Chain Security Report".
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Source: https://blog.aquasec.com/software-supply-chain-attacks-2021
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{D6087671-7D05-7C43-9017-0CE64D4F013B}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-1.2.03. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may deploy a container via Kubernetes dashboard, Kubeflow, and Docker's create and start. The deployed container then can be used to execute malicious commands or download malware. Or to deploy the image with default configurations without network rules and limitations to avoid defense mechanisms of the environment.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Source: https://attack.mitre.org/techniques/T1610/</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{3F3319BE-5CBE-CA40-8178-F0E9F800511B}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-3.1.03.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may modify cloud accounts by adding a new set of credentials. Having adversary-controlled credentials in the cloud accounts allows adversaries to have persistent access to the targeted system. For example, one of the ways to accomplish adding an SSH key is in AWS - using ImportKeyPair or CreateKeyPair API, and in GCP -  gcloud compute os-login ssh-keys add command. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Source: https://attack.mitre.org/techniques/T1098/001/</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{967BAD07-8A1E-174B-8485-9D656780B7F8}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-4.2.03.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may perform a privilege escalation to get admin access to the system. In containerized environments, there are a plethora of ways to conduct a privilege escalation, such as listing secrets to get the admin secret, impersonating a privileged group, exploiting the control plane, for example, Kubernetes API server or kublet, to get access to admin secrets.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Source: https://attack.mitre.org/techniques/T1068/
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>https://blog.lightspin.io/kubernetes-pod-privilege-escalation</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{78C2BA6E-F8C1-4B4F-814D-FF85BD4C49C9}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-5.1.03. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may modify cloud compute infrastructure, that can include creating spanshots, creating, deleting and reverting cloud instances. Modifying infractructure may 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Source: https://attack.mitre.org/techniques/T1578/</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{8CB8BC86-613E-644C-96F5-110DFA369717}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-0.1.04.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>The adversary</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> may try to compromise an application or devise facing the internet to bring unexpected behavior. In cloud baser or containerized environments, it can cause taking advantage of the underlying infrastructure. This makes it possible for adversaries to access container API or container host.  
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Source: https://attack.mitre.org/techniques/T1190/</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{1609E533-69A2-3142-87D5-9EB898DC3C15}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-1.2.04.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may compromise job scheduling in containerized environments. It can be used to schedule the deployment of a container that executes malicious code. Container job scheduling works similarly to the Cron Job in Linux, thus performing defined tasks in a designated time. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">CronJob in Kubernetes can be used to schedule a specific Job, for example, a Job that executes a malicious code in the pods of a cluster.  
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Source: https://attack.mitre.org/techniques/T1053/007/ </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{D519424D-9C9E-8C46-834C-7F846C6BB232}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-3.1.04.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may create a new account to keep persistent access to the target system. In cloud environments, adversaries can add accounts to a specific service to reduce detection risk.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Source: https://attack.mitre.org/techniques/T1136/003/</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{3CD7B2D3-833D-A145-A848-BDA24FC8624E}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-4.2.04.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may compromise job scheduling in containerized environments. It can be used to schedule the deployment of a container that executes malicious code. Container job scheduling works similarly to the Cron Job in Linux, thus performing defined tasks in a designated time. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">CronJob in Kubernetes can be used to schedule a specific Job, for example, a Job that executes a malicious code in the pods of a cluster.  
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Source: https://attack.mitre.org/techniques/T1053/007/ </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{264B6D54-0FCF-CC4B-8E68-5FA3FF02D8F7}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-0.2.05.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may attempt to add a compromised image to the private registry given its access. Or they can add compromised images to a public register, like Docker Hub, and expect the user to use an untrusted image. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/ </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{74D342C9-0AC5-D24B-A773-F8E3CA33114B}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-1.2.05.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may compromise the running SSH server inside on container. Having legitimate credentials gained by phishing or brute-forcing, an adversary may remotely access a container. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{CE6F9465-DA95-C047-8BD8-8E4C1448D89D}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-3.2.05.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may access the system via external remote services (e.g., VPNs), which allows them to connect from the remote location to the system. In the case of containerized environments, there are sensitive interfaces that are not meant to be exposed publicly. But sometimes due to misconfigured environments, they can be exposed. As they don't require authentication adversaries can use them to deploy a container or run malicious code. Examples of those interfaces are Docker API, Kubernetes API server, kublet, Kubeflow. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Source: https://attack.mitre.org/techniques/T1133/ https://www.microsoft.com/security/blog/2021/03/23/secure-containerized-environments-with-updated-threat-matrix-for-kubernetes/
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{DA287239-1E16-D244-83F6-08007E03B6EA}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-4.2.05.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may get access to or deploy a privileged container. A privileged container has permission to do a wide variety of actions on the host. Thus, by gaining access to it, the adversary may modify the host and get access to the admin information and resources and the containers located on the same host. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>https://cloud.redhat.com/blog/protecting-kubernetes-against-mitre-attck-privilege-escalation?extIdCarryOver=true&amp;sc_cid=7013a000002pdO9AAI</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{47AC771D-ED4A-3F46-8518-482257C20A58}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-0.1.06. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may access a kubeconfig file that is exfiltrated, uploaded to the wrong place, or via the compromised client. Having a kubeconfig file gives adversary details about the cluster, such as credentials. Thus, it can be used for accessing the cluster.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/ </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{A96A3AE6-1007-2A4D-B8DB-F779C14F8E4F}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-1.2.06.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may inject a sidecar container in the legitimate pod of the cluster to avoid adding a new pod. In Kubernetes pod is one or a group of containers in the shared network. A sidecar container is a container that exists next to the main container in the pod. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Source: https://www.microsoft.com/security/blog/2021/03/23/secure-containerized-environments-with-updated-threat-matrix-for-kubernetes/ </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{423454CC-9885-1140-B82F-DE20CB3EBB76}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-3.2.06.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may compromise job scheduling in containerized environments. It can be used to schedule the deployment of a container that executes malicious code. Container job scheduling works similarly to the Cron Job in Linux, thus performing defined tasks in a designated time. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">CronJob in Kubernetes can be used to schedule a specific Job, for example, a Job that executes a malicious code in the pods of a cluster.  
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Source: https://attack.mitre.org/techniques/T1053/007/ 
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{409D2166-77B4-B144-83BD-52741F7BB4BA}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-4.2.06.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may create a binding to the privileged or admin role if they gain permission to create bindings. A role binding allows to give permissions specific to the role to the user or group of users and is an initial part of Role-based access control (RBAC) in Kubernetes.   
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Sources: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">https://cloud.redhat.com/blog/protecting-kubernetes-against-mitre-attck-privilege-escalation?extIdCarryOver=true&amp;sc_cid=7013a000002pdO9AAI
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>https://kubernetes.io/docs/reference/access-authn-authz/rbac/</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{2A491A24-E588-9D4A-906E-37997D95454D}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-1.2.07.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{32A56726-D1E4-294B-AEBD-36D761A48D30}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-3.2.07.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may mount a file or folder to a target container using hostPath volume. It's used to mount a file/folder from a host machine to a container and can be exploited by adversaries to get persistent access to the host machine. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{C6DE8D0A-816C-294F-A3FD-E954EE29BB1C}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-1.2.08.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{C039963C-7E3E-DA49-9E95-34011681B474}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-3.2.08.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>The adversary may use Kubernetes controllers (</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Deployments or DaemonSets</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">) to have a constantly running container in the cluster, that can execute a malicious code. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Source: https://cloud.redhat.com/blog/protecting-kubernetes-against-mitre-attck-persistence?extIdCarryOver=true&amp;sc_cid=7013a000002pdO9AAI 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{41A33C7B-CADF-CD41-A300-822D9A98835C}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-1.3.09.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may use an SSH to connect to the CI/CD pipeline. If CI/CD pipeline has allowed SSH access and the adversary gained valid credentials, the adversary can access the CI/CD pipeline servers. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Source: https://github.com/rung/threat-matrix-cicd</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{59E253AB-32BB-204B-B0CC-3CB049805993}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-1.3.10.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may modify CI/CD configurations. When CI/CD configurations on the Git repository are allowed without review, Git allows pushing unsigned commits,  or there is no signature to CI/CD configurations, an adversary can change configurations. Weak audit login can help them remain undetected. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Source: https://github.com/rung/threat-matrix-cicd</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{96B5E9E5-3262-DA49-AE7F-72ECFED4F730}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-1.3.11.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may modify the configuration of the production environment by having valid credentials. For example, when credentials in the system are not rotated regularly and don't follow the least privilege principle, compromising a secret manager and stealing credentials adversary can modify the production environment. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Source: https://github.com/rung/threat-matrix-cicd</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B24" authorId="0" shapeId="0" xr:uid="{BBC4BA4B-DA26-AF42-B82C-A9F7F4632EF2}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-1.3.12.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may exploit the weakest/less secure link in the CI/CD pipeline. Mainly targeted areas are exploits on widely used open-source packages, open-source vulnerabilities, compromised CI/CD tools, and changes in the build process.  
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">In 2021 suply chain attacks increased by 300% compared to 2020 based on the Aqua "2021 Software Supply Chain Security Report".
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Source: https://blog.aquasec.com/software-supply-chain-attacks-2021
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H24" authorId="0" shapeId="0" xr:uid="{878362C0-557F-684D-8DF9-3AF784FEFD6F}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-8.3.13.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may escalate privilages from the CI/CD environment to other comonents of the system, if CI/CD pipeline is not isolated from other systems. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Source: https://github.com/rung/threat-matrix-cicd </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B26" authorId="0" shapeId="0" xr:uid="{D223E137-1FE5-8044-96C1-97441E06D2A9}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-1.3.13.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may deploy modified applications or server images in the production environment by having valid credentials. For example, when credentials in the system are not rotated regularly and don't follow the least privilege principle, compromising a secret manager and stealing credentials, the adversary can deploy modified applications or container images, functions, and VM images to the production environment. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Source: https://github.com/rung/threat-matrix-cicd
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E26" authorId="0" shapeId="0" xr:uid="{1ED8488C-1DC2-E943-B2B0-9949955588EA}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-5.3.13.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may implant a malicious container image into CI/CD pipeline to achieve persistence. Weak audit login can help an adversary remain undetected. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Source: https://github.com/rung/threat-matrix-cicd</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B28" authorId="0" shapeId="0" xr:uid="{A72D13B9-9B5F-FC42-B083-7277EA5C513D}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-1.3.14.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may inject code to IaC configuration, inject source code, or a bad dependency. For example, in the CI stage adversary can change the application to execute a test code on Ci if the policy of code doesn't restrict a dangerous code. Adversaries can inject bad dependency if untrusted libraries and tools are not restricted. And an adversary can inject code to IaC (Infrastructure as code), that is defines as using machine-readable files to manage data centers. For example, via Terraform as it allows code execution and adding of files. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Source: https://github.com/rung/threat-matrix-cicd</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C28" authorId="0" shapeId="0" xr:uid="{527C0F73-64F1-B441-A8FB-F914FC488533}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-3.3.14.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may implant a malicious container image into CI/CD pipeline to achieve persistence. </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Weak audit login can help an adversary remain undetected. </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Source: https://github.com/rung/threat-matrix-cicd</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{24B58332-278C-3C45-ACE9-38CF20F292B4}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-4.3.14.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may escalate privilages from the CI/CD environment to other comonents of the system, if </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>CI/CD pipeline is n</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">ot isolated from other systems. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Source: https://github.com/rung/threat-matrix-cicd </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C30" authorId="0" shapeId="0" xr:uid="{54B1CDBE-3EE4-7149-B7FA-ABF7CFB3F06A}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-3.3.15.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may compromise CI/CD server from a pipeline, espesially if </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">the enviroment created on the pipeline run </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">is not cleaned up after every run. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Source: https://github.com/rung/threat-matrix-cicd</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C32" authorId="0" shapeId="0" xr:uid="{5EC011AE-B08F-5644-96C2-ED7421740754}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-3.3.16.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may modify CI/CD configurations. When CI/CD configurations on the Git repository are allowed without review, Git allows pushing unsigned commits,  or there is no signature to CI/CD configurations, an adversary can change configurations. Weak audit login can help them remain undetected. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Source: https://github.com/rung/threat-matrix-cicd</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C34" authorId="0" shapeId="0" xr:uid="{313B586A-B403-2F4B-B2E2-67BCF43D6013}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">F-3.3.17.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The adversary may inject code to IaC configuration, inject source code, or a bad dependency. For example, in the CI stage adversary can change the application to execute a test code on Ci if the policy of code doesn't restrict a dangerous code. Adversaries can inject bad dependency if untrusted libraries and tools are not restricted. And an adversary can inject code to IaC (Infrastructure as code), that is defines as using machine-readable files to manage data centers. For example, via Terraform as it allows code execution and adding of files. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Source: https://github.com/rung/threat-matrix-cicd
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="253">
   <si>
     <t>Initial Access</t>
   </si>
@@ -2372,38 +221,15 @@
     <t>Writable Volume Mounts on the Host</t>
   </si>
   <si>
-    <t>Images from a Private Registry</t>
-  </si>
-  <si>
     <t>Exploitation for Privilege Escalation</t>
   </si>
   <si>
     <t>Privilleged Container</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> F-1.0.01.
-The adversary may publish a malicious image in the public repository. Adversaries may try to hide the fact that the image is malicious by matching a legitimate name. Thus users might use the image without realizing that it is malicious. This leads to the execution of code that can be used for starting cryptocurrency mining in the instance or container. 
-Source: https://attack.mitre.org/techniques/T1204/003/</t>
-  </si>
-  <si>
-    <t>F-0.0.02.
-The adversary may access the system via external remote services (e.g., VPNs), which allows them to connect from the remote location to the system. In the case of containerized environments, there are sensitive interfaces that are not meant to be exposed publicly. But sometimes due to misconfigured environments, they can be exposed. As they don't require authentication adversaries can use them to deploy a container or run malicious code. Examples of those interfaces are Docker API, Kubernetes API server, kublet, Kubeflow. 
-Source: https://attack.mitre.org/techniques/T1133/ https://www.microsoft.com/security/blog/2021/03/23/secure-containerized-environments-with-updated-threat-matrix-for-kubernetes/</t>
   </si>
   <si>
     <t xml:space="preserve">F-4.2.02.
 The adversary may escape from the container to the host environment, which gives them an access to other containers and/or the underlying host. The main cause of this is typically containerized environments that don't have a separation from the host environment. 
 Source: https://attack.mitre.org/techniques/T1611/  </t>
-  </si>
-  <si>
-    <t>F-1.2.03. 
-The adversary may deploy a container via Kubernetes dashboard, Kubeflow, and Docker's create and start. The deployed container then can be used to execute malicious commands or download malware. Or to deploy the image with default configurations without network rules and limitations to avoid defense mechanisms of the environment.
-Source: https://attack.mitre.org/techniques/T1610/</t>
-  </si>
-  <si>
-    <t>F-3.1.03.
-The adversary may modify cloud accounts by adding a new set of credentials. Having adversary-controlled credentials in the cloud accounts allows adversaries to have persistent access to the targeted system. For example, one of the ways to accomplish adding an SSH key is in AWS - using ImportKeyPair or CreateKeyPair API, and in GCP -  gcloud compute os-login ssh-keys add command. 
-Source: https://attack.mitre.org/techniques/T1098/001/</t>
   </si>
   <si>
     <t>F-4.2.03.
@@ -2412,36 +238,9 @@
 https://blog.lightspin.io/kubernetes-pod-privilege-escalation</t>
   </si>
   <si>
-    <t>F-0.1.04.
-The adversary may try to compromise an application or devise facing the internet to bring unexpected behavior. In cloud baser or containerized environments, it can cause taking advantage of the underlying infrastructure. This makes it possible for adversaries to access container API or container host.  
-Source: https://attack.mitre.org/techniques/T1190/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F-1.2.04.
-The adversary may compromise job scheduling in containerized environments. It can be used to schedule the deployment of a container that executes malicious code. Container job scheduling works similarly to the Cron Job in Linux, thus performing defined tasks in a designated time. 
-CronJob in Kubernetes can be used to schedule a specific Job, for example, a Job that executes a malicious code in the pods of a cluster.  
-Source: https://attack.mitre.org/techniques/T1053/007/ </t>
-  </si>
-  <si>
     <t>F-3.1.04.
 The adversary may create a new account to keep persistent access to the target system. In cloud environments, adversaries can add accounts to a specific service to reduce detection risk.
 Source: https://attack.mitre.org/techniques/T1136/003/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F-4.2.04.
-The adversary may compromise job scheduling in containerized environments. It can be used to schedule the deployment of a container that executes malicious code. Container job scheduling works similarly to the Cron Job in Linux, thus performing defined tasks in a designated time. 
-CronJob in Kubernetes can be used to schedule a specific Job, for example, a Job that executes a malicious code in the pods of a cluster.  
-Source: https://attack.mitre.org/techniques/T1053/007/ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">F-0.2.05.
-The adversary may attempt to add a compromised image to the private registry given its access. Or they can add compromised images to a public register, like Docker Hub, and expect the user to use an untrusted image. 
-Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/ </t>
-  </si>
-  <si>
-    <t>F-1.2.05.
-The adversary may compromise the running SSH server inside on container. Having legitimate credentials gained by phishing or brute-forcing, an adversary may remotely access a container. 
-Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
   </si>
   <si>
     <t xml:space="preserve">F-3.2.05.
@@ -2450,93 +249,27 @@
 </t>
   </si>
   <si>
-    <t>F-4.2.05.
-The adversary may get access to or deploy a privileged container. A privileged container has permission to do a wide variety of actions on the host. Thus, by gaining access to it, the adversary may modify the host and get access to the admin information and resources and the containers located on the same host. 
-Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/
-https://cloud.redhat.com/blog/protecting-kubernetes-against-mitre-attck-privilege-escalation?extIdCarryOver=true&amp;sc_cid=7013a000002pdO9AAI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F-0.1.06. 
-The adversary may access a kubeconfig file that is exfiltrated, uploaded to the wrong place, or via the compromised client. Having a kubeconfig file gives adversary details about the cluster, such as credentials. Thus, it can be used for accessing the cluster.
-Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">F-1.2.06.
-The adversary may inject a sidecar container in the legitimate pod of the cluster to avoid adding a new pod. In Kubernetes pod is one or a group of containers in the shared network. A sidecar container is a container that exists next to the main container in the pod. 
-Source: https://www.microsoft.com/security/blog/2021/03/23/secure-containerized-environments-with-updated-threat-matrix-for-kubernetes/ </t>
-  </si>
-  <si>
-    <t>F-4.2.06.
-The adversary may create a binding to the privileged or admin role if they gain permission to create bindings. A role binding allows to give permissions specific to the role to the user or group of users and is an initial part of Role-based access control (RBAC) in Kubernetes.   
-Sources: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/
-https://cloud.redhat.com/blog/protecting-kubernetes-against-mitre-attck-privilege-escalation?extIdCarryOver=true&amp;sc_cid=7013a000002pdO9AAI
-https://kubernetes.io/docs/reference/access-authn-authz/rbac/</t>
-  </si>
-  <si>
-    <t>F-1.3.09.
-The adversary may use an SSH to connect to the CI/CD pipeline. If CI/CD pipeline has allowed SSH access and the adversary gained valid credentials, the adversary can access the CI/CD pipeline servers. 
-Source: https://github.com/rung/threat-matrix-cicd</t>
-  </si>
-  <si>
     <t xml:space="preserve">F-2.3.17.
 The adversary may inject code to IaC configuration, inject source code, or a bad dependency. For example, in the CI stage adversary can change the application to execute a test code on Ci if the policy of code doesn't restrict a dangerous code. Adversaries can inject bad dependency if untrusted libraries and tools are not restricted. And an adversary can inject code to IaC (Infrastructure as code), that is defines as using machine-readable files to manage data centers. For example, via Terraform as it allows code execution and adding of files. 
 Source: https://github.com/rung/threat-matrix-cicd
 </t>
   </si>
   <si>
-    <t>F-2.3.16.
-The adversary may modify CI/CD configurations. When CI/CD configurations on the Git repository are allowed without review, Git allows pushing unsigned commits,  or there is no signature to CI/CD configurations, an adversary can change configurations. Weak audit login can help them remain undetected. 
-Source: https://github.com/rung/threat-matrix-cicd</t>
-  </si>
-  <si>
     <t>F-2.3.15.
 The adversary may compromise CI/CD server from a pipeline, espesially if the enviroment created on the pipeline run is not cleaned up after every run. 
 Source: https://github.com/rung/threat-matrix-cicd</t>
   </si>
   <si>
-    <t>F-1.3.14.
-The adversary may inject code to IaC configuration, inject source code, or a bad dependency. For example, in the CI stage adversary can change the application to execute a test code on Ci if the policy of code doesn't restrict a dangerous code. Adversaries can inject bad dependency if untrusted libraries and tools are not restricted. And an adversary can inject code to IaC (Infrastructure as code), that is defines as using machine-readable files to manage data centers. For example, via Terraform as it allows code execution and adding of files. 
-Source: https://github.com/rung/threat-matrix-cicd</t>
-  </si>
-  <si>
     <t>F-2.3.14.
 The adversary may implant a malicious container image into CI/CD pipeline to achieve persistence. Weak audit login can help an adversary remain undetected. 
 Source: https://github.com/rung/threat-matrix-cicd</t>
   </si>
   <si>
-    <t xml:space="preserve">F-1.3.13.
-The adversary may deploy modified applications or server images in the production environment by having valid credentials. For example, when credentials in the system are not rotated regularly and don't follow the least privilege principle, compromising a secret manager and stealing credentials, the adversary can deploy modified applications or container images, functions, and VM images to the production environment. 
-Source: https://github.com/rung/threat-matrix-cicd
-</t>
-  </si>
-  <si>
     <t>F-4.3.13.
 The adversary may implant a malicious container image into CI/CD pipeline to achieve persistence. Weak audit login can help an adversary remain undetected. 
 Source: https://github.com/rung/threat-matrix-cicd</t>
   </si>
   <si>
-    <t>F-1.3.10.
-The adversary may modify CI/CD configurations. When CI/CD configurations on the Git repository are allowed without review, Git allows pushing unsigned commits,  or there is no signature to CI/CD configurations, an adversary can change configurations. Weak audit login can help them remain undetected. 
-Source: https://github.com/rung/threat-matrix-cicd</t>
-  </si>
-  <si>
-    <t>F-1.3.11.
-The adversary may modify the configuration of the production environment by having valid credentials. For example, when credentials in the system are not rotated regularly and don't follow the least privilege principle, compromising a secret manager and stealing credentials adversary can modify the production environment. 
-Source: https://github.com/rung/threat-matrix-cicd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F-1.3.12.
-The adversary may exploit the weakest/less secure link in the CI/CD pipeline. Mainly targeted areas are exploits on widely used open-source packages, open-source vulnerabilities, compromised CI/CD tools, and changes in the build process.  
-In 2021 suply chain attacks increased by 300% compared to 2020 based on the Aqua "2021 Software Supply Chain Security Report".
-Source: https://blog.aquasec.com/software-supply-chain-attacks-2021
-</t>
-  </si>
-  <si>
-    <t>F-2.2.07.
-The adversary may mount a file or folder to a target container using hostPath volume. It's used to mount a file/folder from a host machine to a container and can be exploited by adversaries to get persistent access to the host machine. 
-Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
-  </si>
-  <si>
     <t>Valid Accounts</t>
   </si>
   <si>
@@ -2552,12 +285,6 @@
     <t>Impair Defenses</t>
   </si>
   <si>
-    <t xml:space="preserve">F-5.0.02.
-The adversary may turn off, exhaust, or block the defensive mechanisms of a target system. Defensive mechanisms include  security tools, cloud firewalls, or cloud logs. Having these mechanisms disabled allows adversaries to avoid detecting malicious activities and system modification. 
-In cloud environments, modifying cloud firewall rules allow bypassing limitations on accessing cloud resources. 
-Source: https://attack.mitre.org/techniques/T1562/  https://attack.mitre.org/techniques/T1562/007/ </t>
-  </si>
-  <si>
     <t xml:space="preserve">Data from Information Repositories </t>
   </si>
   <si>
@@ -2565,13 +292,6 @@
   </si>
   <si>
     <t>Supply Chain Compromise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F-0.0.03. 
-The adversary may exploit the weakest/less secure link in the CI/CD pipeline or application. Mainly targeted areas are exploits on widely used open-source packages, open-source vulnerabilities, compromised CI/CD tools, and changes in the build process as part of an unpatched or malicious supply chain. 
-In 2021 suply chain attacks increased by 300% compared to 2020 based on the Aqua "2021 Software Supply Chain Security Report".
-Source: https://blog.aquasec.com/software-supply-chain-attacks-2021
- </t>
   </si>
   <si>
     <t>Account Manipulation</t>
@@ -2641,9 +361,6 @@
     <t>Compromised etcd</t>
   </si>
   <si>
-    <t>K8s API Server Vulnerability</t>
-  </si>
-  <si>
     <t>CI/CD Configuration</t>
   </si>
   <si>
@@ -2687,19 +404,6 @@
   </si>
   <si>
     <t>Access Secret Manager</t>
-  </si>
-  <si>
-    <t>F-0.4.01.
-The adversary may use compromised credentials of existing accounts. Obtained certificates may give increased privileges and provide access to restricted network areas. Not using malware can make detecting the presence of an adversary harder.
-Different types of accounts and credentials can be targeted, for example, cloud credentials, default accounts, local accounts, Git repository, CI/CD service, and server hosting Git repository. 
-Source: https://attack.mitre.org/techniques/T1078/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F-3.4.01.
-The adversary may use compromised credentials of existing accounts. Obtained certificates may give increased privileges and provide access to restricted network areas. Not using malware can make detecting the presence of an adversary harder.
-Different types of accounts and credentials can be targeted, for example, cloud credentials, default accounts, local accounts. 
-Source: https://attack.mitre.org/techniques/T1078/
-</t>
   </si>
   <si>
     <t>Modify Production Environment</t>
@@ -2731,45 +435,12 @@
     <t>F-4.2.07.
 The adversary may delete log files or other data that contain signs of adversary presence in the system. This may include clearing container logs, deleting Kubernetes events, etc. Such an activity affects the integrity of the system, as due to the lack of log data, events remain unreported. It also affects the incidence detection, as a lack of data prevents the correct logs correlation from indicating the malicious activity in the system. 
 Source: https://attack.mitre.org/techniques/T1070/</t>
-  </si>
-  <si>
-    <t>F-4.2.08.
-The adversary may change/manipulate the name or metadata of a file/object. Masquerading is used to evade detection. It takes place when malicious files/objects are modified to look legitimate by changing the name and defining a different file type so that the user will misidentify it. Legitimate location can also be matched when applicable. 
-In containerized environments, the adversary may exploit pod/container name similarity. In the case of pods created by controllers, for example, Deployment, they have a random suffix in the name and an unrandom part. So, the adversary can create a pod that will emulate the look of the legitimate pod by using a known part and adding a randomized suffix.  
-Source: https://attack.mitre.org/techniques/T1036/ https://attack.mitre.org/techniques/T1036/005/ https://www.microsoft.com/security/blog/2021/03/23/secure-containerized-environments-with-updated-threat-matrix-for-kubernetes/</t>
   </si>
   <si>
     <t>F-4.2.09.
 The adversary may execute rootkit after mounting /mnt and gaining access to the host with chroot. 
 A rootKit is “a set of programs which patch and trojan existing execution paths within the system”, defined by Greg Hoglund (NT Rootkit author). The rootkit is used to evade detection and get privileged access to the system. The adversary may use LD_PRELOAD to match names of malicious libraries to libraries on the target system, so they are loaded during the program execution.  
 Source: https://info.aquasec.com/cloud-native-threats-aqua https://books.google.fi/books?hl=en&amp;lr=&amp;id=hODFCgAAQBAJ&amp;oi=fnd&amp;pg=PR5&amp;dq=HAnDBOOK+OF+SECURITY+AnD+nETWORKS&amp;ots=H4akui-F1U&amp;sig=jf5Moo9F-mr4xNfCj_pZAQVMz6k&amp;redir_esc=y#v=onepage&amp;q=HAnDBOOK%20OF%20SECURITY%20AnD%20nETWORKS&amp;f=false https://attack.mitre.org/techniques/T1574/006/</t>
-  </si>
-  <si>
-    <t>F-6.2.16.
-(host mounts)
-The adversary may 
-Source:</t>
-  </si>
-  <si>
-    <t>F-6.2.15.
-(sensitive RBAC)
-The adversary may 
-Source:</t>
-  </si>
-  <si>
-    <t>F-7.2.10.
-The adversary may 
-Source:</t>
-  </si>
-  <si>
-    <t>F-9.2.04.
-The adversary may 
-Source:</t>
-  </si>
-  <si>
-    <t>F-1.2.07.
-The adversary may 
-Source:</t>
   </si>
   <si>
     <t>Steal Application Access Token</t>
@@ -2800,9 +471,6 @@
     </r>
   </si>
   <si>
-    <t>Injection to IaC Configuration, to Source Code, Bad Dependency</t>
-  </si>
-  <si>
     <t>Access Host Filesystem</t>
   </si>
   <si>
@@ -2835,13 +503,6 @@
 Source: https://attack.mitre.org/techniques/T1552/ https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
   </si>
   <si>
-    <t>F-6.0.02.
-The adversary may brute force system credentials to get access to the system. The attacker can perform brute force online by guessing a password to the system and receiving an instant result about their validity, or an offline, by using previously obtained hashes. The adversary may use the knowledge gathered in other steps, such as valid accounts, account and password policy discovery. Having the following data decreases the time needed to brute force valid credentials.
-Password spraying is one of the common techniques. The attacker uses a list of the most common password that matches a password policy of the environment (if known) and uses it as a possible list of user passwords. Then, to avoid being blocked for too many failed log ins, the attacker can target several accounts in the system. 
-Another common technique is credential stuffing. The adversary may look for leaked credentials on the web and access the system by credential overlap. For example, sometimes users use the same password for personal and professional use (credential overlap), so adversaries may access a target system using a leaked personal password. 
-Source: https://attack.mitre.org/techniques/T1110/ https://attack.mitre.org/techniques/T1110/001/ https://attack.mitre.org/techniques/T1110/003/ https://attack.mitre.org/techniques/T1110/004/</t>
-  </si>
-  <si>
     <t>F-6.1.05.
 The adversary may steal a web session cookie to access systems and applications without the need for credentials. Session cookies keep a user authenticated to a website. Here cookie is an authentication token after they complete the first authentication. Session cookie stays valid even when the user is not actively using the application. It can be found in various locations as a disk or network traffic or can be stolen using malware on a local system web browser or collected on the proxy. After stealing a web session cookie, the adversary can use it to authenticate a target system as alternate authentication material (F-5.1.05.). 
 Source: https://attack.mitre.org/techniques/T1539/</t>
@@ -2865,11 +526,6 @@
 Source: https://github.com/rung/threat-matrix-cicd</t>
   </si>
   <si>
-    <t>F-7.0.01.
-The adversary may scan network services to discover services running on remote hosts or scan for vulnerabilities. Some of the discovered services may be vulnerable, which can be used for exploitation. An adversary may discover services running on other than a target machine cloud hosts in cloud-based systems. Moreover, if the on-premise environment is connected to the cloud host, the adversary may be able to discover services on the premice host. In the case of containerized systems, the adversary with access to one container can map all networks, as, by default, there are no limitations on pods communication.   
-Source: https://attack.mitre.org/techniques/T1046/ https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
-  </si>
-  <si>
     <t>F-7.0.02.
 The adversary may try to discover user groups and permissions. Knowledge of user groups and permission settings helps the adversary determine a particular user in the groups and groups and users with elevated permissions. The adversary may gather permission groups through API interfaces in cloud environments, such as Azure CLI and Google Cloud Identity Provider API. 
 Source: https://attack.mitre.org/techniques/T1069/ https://attack.mitre.org/techniques/T1069/003/</t>
@@ -2885,11 +541,6 @@
 Source: https://attack.mitre.org/techniques/T1087/ https://attack.mitre.org/techniques/T1087/004/</t>
   </si>
   <si>
-    <t>F-7.1.04.
-The adversary may try to discover components of Infrastructure-As-a-Service (IaaS) environments using cloud APIs and CLIs. System components include cloud instances, snapshots, virtual machines, and cloud services. APIs and CLI commands have the capability of requesting information about the infrastructure. For example, AWS - ListBuckets - returns buckets owned by the request sender. GCP Cloud SDK CLI - has commands for listing project Google Compute Engine instances. CLI in Azure has commands for displaying details of virtual machines. The adversary can use the gathered information for planning the next attack steps. 
-Source: https://attack.mitre.org/techniques/T1580/</t>
-  </si>
-  <si>
     <t>F-7.1.05.
 The adversary may use cloud or container service account dashboard GUI, accessing it with stolen credentials, to discover information about the system. Such information may include services, resources, and features of the system. The advantage of an enumeration system using GUI rather than API is that the adversary doesn't have to make any API requests. 
 Source: https://attack.mitre.org/techniques/T1538/ https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
@@ -2943,15 +594,6 @@
     <t>Access the Kubernetes or Kubelet API</t>
   </si>
   <si>
-    <t xml:space="preserve">F-1.2.02. 
-The adversary may compromise the container administration services such as kublet, the Kubernetes API server, and the Docker daemon. This can allow them to remotely manage containers in the environment and execute commands. For example, in Docker, the docker exec can be used to execute commands in the running container. In the Kubernetes, execution of commands can be gained by using kubectl exec, the kublet, the Kubernetes API server, and having a proper access level.
-Command for Kubernetes: 
-kubectl exec 
-To run a terminal inside the running conainer: 
-kubectl exec --stdin --tty &lt;name-of-the-pod&gt;  -- /bin/bash
-Source: https://attack.mitre.org/techniques/T1609/ </t>
-  </si>
-  <si>
     <t>F-6.0.04.
 The adversary may steal an application access token to gain access to the remote system or application. It usually requires action from the user side, as tokens are typically acquired through social engineering. Application access tokens are used in the applications to make requests to the API server on behalf of the user and then to gain access to cloud-based applications. OAuth is a common framework used for access delegation. It issues tokens for granting access to the system to users without sharing user password with a system. An adversary may build a malicious website to steal a target user access token.
 Source: https://attack.mitre.org/techniques/T1528/</t>
@@ -2972,9 +614,6 @@
     <t>Automated Collection</t>
   </si>
   <si>
-    <t xml:space="preserve">    </t>
-  </si>
-  <si>
     <t>F-6.1.17.
 The adversary may perform network sniffing of the traffic to get information about the system, users, and authentication details. Network sniffing is monitoring wireless or wired networks to record data. User credentials are one of the biggest targets, especially when transmitted using unencrypted protocols. The adversary may also discover system configurations that are helpful for the consequent attack steps. In the cloud environments, the adversary may utilize AWS Traffic Mirroring, GCP Packet Mirroring, and Azure vTap to record traffic.
 Source: https://attack.mitre.org/techniques/T1040/</t>
@@ -2995,11 +634,6 @@
 Source: https://attack.mitre.org/techniques/T1550/ https://attack.mitre.org/techniques/T1550/004/ https://attack.mitre.org/techniques/T1550/001/</t>
   </si>
   <si>
-    <t>F-8.0.01.
-The adversary may use alternate authentication material to access the target system. For example, web session cookies are commonly used in cloud web applications. Session cookie keeps the user logged in to the application, even when application is not actively used. Thus, the adversary may steal a cookie to bypass the log in and access the data available to the victim user. In containerized environments, secrets, including application credentials, can be stored in the configuration files.
-Source: https://attack.mitre.org/techniques/T1550/ https://attack.mitre.org/techniques/T1550/004/ https://attack.mitre.org/techniques/T1550/001/ https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
-  </si>
-  <si>
     <t>F-8.1.02.
 The adversary may exploit a trusted account in the system to perform a phishing attack with a higher likelihood of the target opening it. In this attack, the adversary attempt to capture credentials or spread malware in the system, for example, by using a spearphishing attachment or link. 
 Source: https://attack.mitre.org/techniques/T1534/</t>
@@ -3013,11 +647,6 @@
 Source: https://attack.mitre.org/techniques/T1080/</t>
   </si>
   <si>
-    <t>F-8.2.04.
-The adversary may escape from the exploited container to the underlying system by creating a container with a  writable hostPath volume, that later can be used for escapint to the host. 
-Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
-  </si>
-  <si>
     <t xml:space="preserve">F-8.3.12.
 The adversary may escalate privileges from the CI/CD environment to other components of the system, if CI/CD pipeline is not isolated from other systems. 
 Source: https://github.com/rung/threat-matrix-cicd </t>
@@ -3046,31 +675,7 @@
 Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
   </si>
   <si>
-    <t>F-3.2.07.
-(metadata attack via workload identity)
-The adversary may leverage the access from a container to the other cloud resources. The adversary can access the service principal file(used to create and manage resources), steal its credentials, and utilize them to modify or view cloud resources. 
-Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
-  </si>
-  <si>
-    <t>F-7.2.08.
-(workload identity and cloud integrations)
-The adversary may leverage the access from a container to the other cloud resources. The adversary can access the service principal file(used to create and manage resources), steal its credentials, and utilize them to modify or view cloud resources. 
-Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
-  </si>
-  <si>
-    <t>F-2.2.10.
-(postStart and preStop events in pod YAML)
-The adversary may modify container lifecycle hooks to a pod by editing a pod YAML file and changeing postStart and preStop events. Those events can contain a malicious script.  Logs of the Hook handler are not exposed to Pod events. 
-Source: Hacking Kubernetes
-By Andrew Martin, Michael Hausenblas.  https://kubernetes.io/docs/concepts/containers/container-lifecycle-hooks/</t>
-  </si>
-  <si>
     <t>Cluster-Admin Binding</t>
-  </si>
-  <si>
-    <t>F-7.2.09.
-The adversary may attack other containers in the cluster utilizing allowed network traffic between pods. To perform this technique, an adversary have to have access to at least one container in the cluster. . 
-Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
   </si>
   <si>
     <t>F-7.3.11.
@@ -3083,21 +688,6 @@
 Source: https://attack.mitre.org/techniques/T1213/</t>
   </si>
   <si>
-    <t>F-9.1.03.
-The adversary may stage data in a staging area ( specific location in the system)  before exfiltration it. The adversary can stage data to a particular instance or a virtual machine in cloud environments. 
-Source: https://attack.mitre.org/techniques/T1074/</t>
-  </si>
-  <si>
-    <t>F-9.1.05.
-The adversary may collect internal data using automatic data gathering techniques. The adversary may use cloud APIs, command-line interfaces, or transform services to collect information in the cloud environments automatically. 
-Source: https://attack.mitre.org/techniques/T1119/</t>
-  </si>
-  <si>
-    <t>F-10.1.01.
-The adversary may exfiltrate data and backups from one cloud account to another within the same cloud provider to avoid detection. This transfer within the same cloud provider can be not monitored, unlike data transfers over external network interfaces. 
-Source :https://attack.mitre.org/techniques/T1537/</t>
-  </si>
-  <si>
     <t>F-10.1.02.
 The adversary may exfiltrate data using existing command and control channels. The data that have to be exfiltrated may be encoded into the communication channels using the same protocol as C2 communicators.  
 Source: https://attack.mitre.org/techniques/T1041/</t>
@@ -3113,26 +703,6 @@
 Source: https://github.com/rung/threat-matrix-cicd </t>
   </si>
   <si>
-    <t>F-9.1.01.
-The adversary may collect information from the cloud data storage that does not have a proper protection level. For example, cloud data storage does not have running applications, and their data can be retrieved via APIs. Commonly the end-users misconfigure such storage, leaving them unproperly secured. Or credentials gathered in the previous steps can be used for accessing storage with access permissions controls. 
-Source: https://attack.mitre.org/techniques/T1530/</t>
-  </si>
-  <si>
-    <t>F-11.0.01.
-The adversary may destroy information in the system to interrupt its availability. This can be achieved by deleting cloud storage, cloud storage accounts, or other infrastructure in the cloud environments. 
-Source: https://attack.mitre.org/techniques/T1485/</t>
-  </si>
-  <si>
-    <t>F-11.4.02.
-The adversary may perform a Denial-of-Service (DoS) attack to make services unavailable to users. A DoS is an attack that causes a machine or network to be inaccessible to the intended users. There are many possible DoS attack types: Endpoint DoS,  Network DoS, Application DoS, Node scheduling DoS, Service discovery DoS, SOC/SIEM DoS. 
-Source:  https://attack.mitre.org/techniques/T1498/ https://attack.mitre.org/techniques/T1499/ https://github.com/rung/threat-matrix-cicd https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
-  </si>
-  <si>
-    <t>F-11.0.03. 
-The adversary may use the system to solve resource-intensive problems, likely affecting systems availability. The most common use case is to mine cryptocurrencies. Cloud-based systems are a common target for this attack, as they have a high potential of available resources. Containerized environments are also commonly targeted via exposed APIs and scaling possibilities.  
-Source: https://attack.mitre.org/techniques/T1496/</t>
-  </si>
-  <si>
     <t>F-11.1.04.
 The adversary may encrypt the data of the system to impact its availability and remove the decryption key from the system. This is usually done to request monetary compensation in exchange for the decryption of the information. In the case of cloud environments, storage objects that belong to compromised accounts can be encrypted. 
 Source: https://attack.mitre.org/techniques/T1486/</t>
@@ -3148,161 +718,428 @@
 Source: https://attack.mitre.org/techniques/T1531/</t>
   </si>
   <si>
-    <t>F-0.3.09.
-(missing auth)
-The adversary may 
-Source: Hacking Kubernetes
-By Andrew Martin, Michael Hausenblas.  https://kubernetes.io/docs/concepts/containers/container-lifecycle-hooks/</t>
-  </si>
-  <si>
-    <t>F-0.2.07.
-(2FA and federating auth mitigate)
-The adversary may 
-Source: Hacking Kubernetes
-By Andrew Martin, Michael Hausenblas.  https://kubernetes.io/docs/concepts/containers/container-lifecycle-hooks/</t>
-  </si>
-  <si>
-    <t>F-0.2.08.
-The adversary may compromise a host utilizing credentials leak, stuffing, or by performing a supply chain compromise, thus using the least secured link in the system, such as unpatched services.
-Source: Hacking Kubernetes
-By Andrew Martin, Michael Hausenblas.  https://kubernetes.io/docs/concepts/containers/container-lifecycle-hooks/</t>
-  </si>
-  <si>
-    <t>F-1.2.08.
-The adversary may add container lifecycle hooks to a pod by editing a pod YAML file and adding postStart and preStop events. Those events can contain a malicious script.  Logs of the Hook handler are not exposed to Pod events. 
-Source: Hacking Kubernetes
-By Andrew Martin, Michael Hausenblas.  https://kubernetes.io/docs/concepts/containers/container-lifecycle-hooks/</t>
-  </si>
-  <si>
-    <t>F-0.2.10.
-(needs CVE and unpatched API server)
-The adversary may 
-Source: Hacking Kubernetes
-By Andrew Martin, Michael Hausenblas.  https://kubernetes.io/docs/concepts/containers/container-lifecycle-hooks/</t>
-  </si>
-  <si>
-    <t>F-2.2.11.
-(exec into and reverse shell in container)
-The adversary may 
-Source: Hacking Kubernetes
-By Andrew Martin, Michael Hausenblas.  https://kubernetes.io/docs/concepts/containers/container-lifecycle-hooks/</t>
-  </si>
-  <si>
-    <t>F-2.2.12.
-(privileged RBAC, reverse shell)
-The adversary may 
-Source: Hacking Kubernetes
-By Andrew Martin, Michael Hausenblas.  https://kubernetes.io/docs/concepts/containers/container-lifecycle-hooks/</t>
-  </si>
-  <si>
-    <t>F-2.2.13.
-(secondary cluster running on compromised nodes)
-The adversary may 
-Source: Hacking Kubernetes
-By Andrew Martin, Michael Hausenblas.  https://kubernetes.io/docs/concepts/containers/container-lifecycle-hooks/</t>
-  </si>
-  <si>
-    <t>F-2.2.09.
-(reverse shell, shadow API server to read audit-log-only headers)
-The adversary may 
-Source: Hacking Kubernetes
-By Andrew Martin, Michael Hausenblas.  https://kubernetes.io/docs/concepts/containers/container-lifecycle-hooks/</t>
-  </si>
-  <si>
-    <t>F-2.2.08.
-The adversary may use Kubernetes controllers (Deployments or DaemonSets) to have a constantly running container in the cluster, that can execute a malicious code. 
-Source: https://cloud.redhat.com/blog/protecting-kubernetes-against-mitre-attck-persistence?extIdCarryOver=true&amp;sc_cid=7013a000002pdO9AAI 
-https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
-  </si>
-  <si>
-    <t>F-3.2.08.
-(logs to container breakout)
-The adversary may 
-Source: Hacking Kubernetes
-By Andrew Martin, Michael Hausenblas.  https://kubernetes.io/docs/concepts/containers/container-lifecycle-hooks/</t>
-  </si>
-  <si>
-    <t>F-3.2.09.
-(stolen credentials, node label rebinding attack)
-The adversary may 
-Source: Hacking Kubernetes
-By Andrew Martin, Michael Hausenblas.  https://kubernetes.io/docs/concepts/containers/container-lifecycle-hooks/</t>
-  </si>
-  <si>
-    <t>F-3.2.10.
-(keys in Secrets, cloud or control plane credentials)
-The adversary may 
-Source: Hacking Kubernetes
-By Andrew Martin, Michael Hausenblas.  https://kubernetes.io/docs/concepts/containers/container-lifecycle-hooks/</t>
-  </si>
-  <si>
-    <t>F-3.2.11.
-(reconfigure and bypass to allow blocked image with flag)
-The adversary may 
-Source: Hacking Kubernetes
-By Andrew Martin, Michael Hausenblas.  https://kubernetes.io/docs/concepts/containers/container-lifecycle-hooks/</t>
-  </si>
-  <si>
-    <t>F-3.2.12.
-(compromise flux and read any Secrets)
-The adversary may 
-Source: Hacking Kubernetes
-By Andrew Martin, Michael Hausenblas.  https://kubernetes.io/docs/concepts/containers/container-lifecycle-hooks/</t>
-  </si>
-  <si>
-    <t>F-3.2.13.
-(kernel or runtime vulnerability e.g., DirtyCOW, `/proc/self/exe`, eBPF verifier bugs, Netfilter)
-The adversary may 
-Source: Hacking Kubernetes
-By Andrew Martin, Michael Hausenblas.  https://kubernetes.io/docs/concepts/containers/container-lifecycle-hooks/</t>
-  </si>
-  <si>
-    <t>F-4.2.10.
-(to cover source IP, external to cluster)
-The adversary may 
-Source: Hacking Kubernetes
-By Andrew Martin, Michael Hausenblas.  https://kubernetes.io/docs/concepts/containers/container-lifecycle-hooks/</t>
-  </si>
-  <si>
-    <t>F-4.2.11.
-(DNS tunneling/exfiltration)
-The adversary may 
-Source: Hacking Kubernetes
-By Andrew Martin, Michael Hausenblas.  https://kubernetes.io/docs/concepts/containers/container-lifecycle-hooks/</t>
-  </si>
-  <si>
-    <t>F-4.2.12.
-The adversary may 
-Source: Hacking Kubernetes
-By Andrew Martin, Michael Hausenblas.  https://kubernetes.io/docs/concepts/containers/container-lifecycle-hooks/</t>
-  </si>
-  <si>
-    <t>F-11.2.06.
-(cluster or cloud datastores, local accounts)
-The adversary may 
-Source: Hacking Kubernetes
-By Andrew Martin, Michael Hausenblas.  https://kubernetes.io/docs/concepts/containers/container-lifecycle-hooks/</t>
-  </si>
-  <si>
-    <t>F-4.4.15.
-The adversary may modify the approver list in Git, given the admin permission on the Git repository service account. This may affect the system if the multi-party approval is not mandatory and the admin list is not limited.
+    <t xml:space="preserve">F-1.1.06. 
+The adversary may access a kubeconfig file that is exfiltrated, uploaded to the wrong place, or via the compromised client. Having a kubeconfig file gives adversary details about the cluster, such as credentials. Thus, it can be used for accessing the cluster.
+Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/ </t>
+  </si>
+  <si>
+    <t>F-2.3.09.
+The adversary may use an SSH to connect to the CI/CD pipeline. If CI/CD pipeline has allowed SSH access and the adversary gained valid credentials, the adversary can access the CI/CD pipeline servers. 
 Source: https://github.com/rung/threat-matrix-cicd</t>
   </si>
   <si>
+    <t>F-2.3.10.
+The adversary may modify CI/CD configurations. When CI/CD configurations on the Git repository are allowed without review, Git allows pushing unsigned commits,  or there is no signature to CI/CD configurations, an adversary can change configurations. Weak audit login can help them remain undetected. 
+Source: https://github.com/rung/threat-matrix-cicd</t>
+  </si>
+  <si>
+    <t>F-2.3.11.
+The adversary may modify the configuration of the production environment by having valid credentials. For example, when credentials in the system are not rotated regularly and don't follow the least privilege principle, compromising a secret manager and stealing credentials adversary can modify the production environment. 
+Source: https://github.com/rung/threat-matrix-cicd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F-2.3.13.
+The adversary may deploy modified applications or server images in the production environment by having valid credentials. For example, when credentials in the system are not rotated regularly and don't follow the least privilege principle, compromising a secret manager and stealing credentials, the adversary can deploy modified applications or container images, functions, and VM images to the production environment. 
+Source: https://github.com/rung/threat-matrix-cicd
+</t>
+  </si>
+  <si>
+    <t>F-2.3.14.
+The adversary may inject code to IaC configuration, inject source code, or a bad dependency. For example, in the CI stage adversary can change the application to execute a test code on Ci if the policy of code doesn't restrict a dangerous code. Adversaries can inject bad dependency if untrusted libraries and tools are not restricted. And an adversary can inject code to IaC (Infrastructure as code), that is defines as using machine-readable files to manage data centers. For example, via Terraform as it allows code execution and adding of files. 
+Source: https://github.com/rung/threat-matrix-cicd</t>
+  </si>
+  <si>
+    <t>F-11.0.01.
+The adversary may destroy information in the system to interrupt its availability. This can be achieved by deleting cloud storage, cloud storage accounts, or other infrastructure in the cloud or containerized environments. 
+Source: https://attack.mitre.org/techniques/T1485/</t>
+  </si>
+  <si>
+    <t>F-1.4.01.
+The adversary may use compromised credentials of existing accounts. Obtained certificates can be used to get increased privileges in the system and provide access to restricted network areas. 
+Different types of accounts and credentials can be targeted. For example: cloud credentials, default accounts, local accounts, Git repository, CI\CD service, and server hosting Git repository 
+Source: https://attack.mitre.org/techniques/T1078/
+ https://www.microsoft.com/security/blog/2021/03/23/secure-containerized-environments-with-updated-threat-matrix-for-kubernetes/
+ https://github.com/rung/threat-matrix-cicd</t>
+  </si>
+  <si>
     <t xml:space="preserve">F-5.4.01.
-The adversary may use compromised credentials of existing accounts. Obtained certificates may give increased privileges and provide access to restricted network areas. Not using malware can make detecting the presence of an adversary harder.
+The adversary may use compromised credentials of existing accounts. Obtained certificates can be used to get increased privileges in the system and provide access to restricted network areas. 
 Different types of accounts and credentials can be targeted, for example, cloud credentials, default accounts, local accounts.
 Source: https://attack.mitre.org/techniques/T1078/
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F-3.4.01.
+The adversary may use compromised credentials of existing accounts. Obtained certificates can be used to get increased privileges in the system and provide access to restricted network areas. 
+Different types of accounts and credentials can be targeted. For example: cloud credentials, default accounts, local accounts, Git repository, CI\CD service, and server hosting Git repository.
+Source: https://attack.mitre.org/techniques/T1078/
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F-1.0.03. 
+The adversary may exploit the weakest/less secure link in the CI/CD pipeline or application. Mainly targeted areas are exploits on widely used open-source packages, open-source vulnerabilities, compromised CI/CD tools, and changes in the build process as part of an unpatched or malicious supply chain.
+In 2021 suply chain attacks increased by 300% compared to 2020 based on the Aqua "2021 Software Supply Chain Security Report".
+Source: https://blog.aquasec.com/software-supply-chain-attacks-2021 
+ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">F-1.2.05.
+The adversary may attempt to add a compromised image to the private registry given its access. Or they can add compromised images to a public register, like Docker Hub, and expect the user to use this compromised image.
+Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/ </t>
+  </si>
+  <si>
+    <t>F-2.2.03. 
+The adversary may deploy a container via Kubernetes dashboard, Kubeflow, or via Kubernetes api server. The deployed container then can be used to execute malicious commands or download malware. Another important aspect of malicious containers is that it allows wider range of techniques to be used and to achieve persistence. 
+Source: https://attack.mitre.org/techniques/T1610/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F-2.2.04.
+The adversary may compromise job scheduling in containerized environments. It can be used to schedule the deployment of a container that executes malicious code. Container job scheduling works similarly to the Cron job in Linux, thus performing defined tasks in a designated time. 
+CronJob in Kubernetes can be used to schedule a specific Job. For example, a Job that executes a malicious code in the Pod of a cluster.
+Source: https://attack.mitre.org/techniques/T1053/007/ </t>
+  </si>
+  <si>
+    <t>F-3.1.03.
+The adversary may modify cloud accounts by adding a new set of credentials. Having adversary-controlled credentials in the cloud accounts allows adversaries to have persistent access to the targeted system. There are several ways to add SSH key in the cloud environment. For example, using ImportKeyPair or CreateKeyPair API in AWS , or gcloud compute os-login ssh-keys add command in GCP.
+Source: https://attack.mitre.org/techniques/T1098/001/</t>
+  </si>
+  <si>
+    <t>F-2.2.07.
+The adversary may mount a file or folder to a target container using hostPath volume. It's used to mount a file/folder from a host machine to a container and can be exploited by adversaries to get persistent access to the host machine.
+Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
+  </si>
+  <si>
+    <t>F-2.3.16.
+The adversary may try to modify CI/CD configurations. When CI/CD configurations on the Git repository are allowed without review, Git allows pushing unsigned commits. When there is no signature to CI/CD configurations, an adversary can try to change configurations. Weak audit login can help an adversary to remain undetected.
+Source: https://github.com/rung/threat-matrix-cicd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F-5.0.02.
+The adversary may turn off, exhaust, or block the defensive mechanisms of a target system. Defensive mechanisms include  security tools, cloud firewalls, or cloud logs. Having these mechanisms disabled allows adversaries to avoid detecting malicious activities and system modification.
+In cloud environments, modifying cloud firewall rules allow bypassing limitations on accessing cloud resources. 
+Source: https://attack.mitre.org/techniques/T1562/  https://attack.mitre.org/techniques/T1562/007/ </t>
+  </si>
+  <si>
+    <t>F-4.2.08.
+The adversary may change/manipulate the name or metadata of a file/object. Masquerading is used to evade detection. It takes place when malicious files/objects are modified to look legitimate by changing the name and defining a different file type so that the user will misidentify it. Legitimate location can also be matched when applicable.
+In containerized environments, the adversary may exploit Pod/container name similarity. Kubernetes system Pods names are appended by a random suffix. Thus, the adversary can create a Pod that will emulate the look of the legitimate pod by using a known Pod name and adding a random suffix.  
+Source: https://attack.mitre.org/techniques/T1036/ https://attack.mitre.org/techniques/T1036/005/ https://www.microsoft.com/security/blog/2021/03/23/secure-containerized-environments-with-updated-threat-matrix-for-kubernetes/</t>
+  </si>
+  <si>
+    <t>F-6.0.02.
+The adversary may brute force system credentials to get access to the system. The adversary can perform brute force online by guessing a password to the system and receiving an instant result about their validity, or offline, by using previously obtained hashes. In addition, the adversary may use the knowledge gathered in other steps, such as valid accounts and account and password policy discovery. Having information about password policy decreases the time needed to brute force valid credentials.
+Source: 
+https://attack.mitre.org/techniques/T1110/
+https://attack.mitre.org/techniques/T1110/001/
+https://attack.mitre.org/techniques/T1110/003/
+https://attack.mitre.org/techniques/T1110/004/</t>
+  </si>
+  <si>
+    <t>F-7.0.01.
+The adversary may scan network to discover running services or remote hosts. Some of the discovered services may be vulnerable, which can be used for exploitation. An adversary may discover services running on other than a target machine. Service discovery from the cloud host may allow an adversary to discover services of the underlying host. In the case of containerized systems, the adversary with access to one container might be able to map all networks, as, by default, there are no limitations on Pods communication.   
+Source: https://attack.mitre.org/techniques/T1046/ https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
+  </si>
+  <si>
+    <t>F-7.0.04.
+The adversary may try to discover components of Infrastructure-As-a-Service (IaaS) environments using cloud APIs and CLIs. System components include cloud instances, snapshots, virtual machines, and cloud services. APIs and CLI commands have the capability of requesting information about the infrastructure. 
+The adversary can use the gathered information for planning the next attack steps. 
+Source: https://attack.mitre.org/techniques/T1580/</t>
+  </si>
+  <si>
+    <t>F-8.2.04.
+The adversary may escape from the exploited container to the underlying system by creating a container with a  writable hostPath volume. Escaping the container will give the adversary access to the host system (underlying system in the containerized environments).
+Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
+  </si>
+  <si>
+    <t>F-9.1.01.
+The adversary may collect information from the cloud data storage that does not have a proper protection. For example, retrieving data from cloud storage directly via unsecured APIs. Commonly the end-users misconfigure such storage, leaving them unsecure. Credentials gathered in the previous steps can be used for accessing storage with access permissions controls.
+Source: https://attack.mitre.org/techniques/T1530/</t>
+  </si>
+  <si>
+    <t>F-11.0.03. 
+The adversary may use the system to solve resource-intensive problems, likely affecting systems availability. The common use case is cryptojacking. Cryptojacking is an act of mining cryptocurrencies. Cloud-based systems are a common target for this attack, as they have a high potential of available resources.  Containerized environments are also commonly targeted via exposed APIs and because of scaling possibilities.  
+Source: https://attack.mitre.org/techniques/T1496/</t>
+  </si>
+  <si>
+    <t>F-11.4.02.
+The adversary may perform a Denial-of-Service (DoS) attack to make services unavailable to users. A DoS is an attack that is intended to cause a machine or network to be inaccessible to the intended users. There are many possible DoS attack types: Endpoint DoS,  Network DoS, Application DoS, Node scheduling DoS, Service discovery DoS, SOC/SIEM DoS. 
+Source:  https://attack.mitre.org/techniques/T1498/ https://attack.mitre.org/techniques/T1499/ https://github.com/rung/threat-matrix-cicd https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
+  </si>
+  <si>
+    <t>F-1.2.07.
+The adversary may try to compromise a user endpoint. Disabled two-factor authentication or not using federated authentication makes it easier for the adversary to perform this technique.
+Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t>F-2.2.08.
+The adversary may use Kubernetes controllers (Deployments or DaemonSets) to have a constantly running container in the cluster, that can execute a malicious code. 
+Source: https://cloud.redhat.com/blog/protecting-kubernetes-against-mitre-attck-persistence
+https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
+  </si>
+  <si>
+    <t>F-4.2.05.
+The adversary may get access to or deploy a privileged container. A privileged container has permission to do a wide variety of actions on the host. Thus, by having access to it, the adversary may modify the host and get access to the admin information and resources located on the same host.
+Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/
+https://cloud.redhat.com/blog/protecting-kubernetes-against-mitre-attck-privilege-escalation</t>
+  </si>
+  <si>
+    <t>F-4.2.06.
+The adversary may create a binding to the privileged or admin role. A role binding allows to give permissions specific to the role to the user or group of users and is an initial part of Role-based access control (RBAC) in Kubernetes.
+Sources: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/
+https://cloud.redhat.com/blog/protecting-kubernetes-against-mitre-attck-privilege-escalation
+https://kubernetes.io/docs/reference/access-authn-authz/rbac/</t>
+  </si>
+  <si>
+    <t>F-1.2.3.09.
+The adversary may access the unsecured etcd cluster. Some etcd clusters have no authentication and are open to the internet. Anyone with access to it can dump all keys using:
+curl http://&lt;ip address&gt;:2379/v2/keys/?recursive=true
+Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t>API Server Vulnerability</t>
+  </si>
+  <si>
+    <t>F-1.2.10.
+The adversary may try to exploit the Kubernetes API server vulnerability. For example, a discovered CVE might be present in the unpatched API server, and an adversary may try to exploit it. 
+Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t>F-2.2.08.
+The adversary may add container lifecycle hooks to a Pod by editing a Pod YAML file and adding, for example, postStart and preStop events. Those events can contain a malicious script. 
+Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/ https://kubernetes.io/docs/concepts/containers/container-lifecycle-hooks/</t>
+  </si>
+  <si>
+    <t>Injection to IaC Configuration, to Source Code, Bad Dependency
+CI/CD</t>
+  </si>
+  <si>
+    <t>F-4.3.16.
+The adversary may bypass a Git repository review. This may affect the system if additional review for approval to trigger deploy on CI/CD pipeline is not required, and/or admin has a permission to push into the main Git repository branch without a review. 
+Source: https://github.com/rung/threat-matrix-cicd</t>
+  </si>
+  <si>
+    <t>F-2.2.10.
+The adversary may modify container lifecycle hooks to a pod by editing a pod YAML file and changeing postStart and preStop events. Those events can contain a malicious script.  Logs of the Hook handler are not exposed to Pod events. 
+Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t>F-2.2.09.
+The adversary may try to exploit a static Pod. An adversary can establish a reverse shell or read audit-log-only headers from the shadow API server.
+Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t>F-2.2.11.
+The adversary may try to rewrite the liveness probes of the Pod. They may exec into the container and establish a reverse shell to modify the liveness probes of the container.
+Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t>F-2.2.12.
+The adversary may try to exploit a shadow Admission control or API server.  They may establish a privileged RBAC to get a reverse shell or exploit vulnerable kube-apiserver versions to change the admission controller validation rules. For example, changing the changeAllowed label to true allows bypassing the admission controller validation rules, permitting any changes on the cluster nodes without validation. 
+Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t>F-2.2.13.
+The adversary may try to establish a K3d botnet. This can be achieved by deploying a secondary cluster running on compromised nodes.
+Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t>F-3.2.08.
+The adversary may try to mount a file or folder to a target container using hostPath volume. It's used to mount a file/folder from a host machine to a container Pod.
+Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t>F-3.2.10.
+The adversary may try to perform a control plane to cloud escalation. Keys in Secrets or cloud or control plane credentials can be used for the technique execution. 
+Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t>F-3.2.11.
+(reconfigure and bypass to allow blocked image with flag)
+The adversary may try to compromise admission controller. They can try to reconfigure or bypass the admission controller to allow blocked image with flag.
+Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t>F-3.2.12.
+The adversary may try to compromise Kubernetes operator. They may attempt to compromise flux and read any Secrets.
+Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t>F-3.2.13.
+The adversary may try to perform a container breakout by exploiting a kernel or runtime vulnerability e.g., DirtyCOW, `/proc/self/exe`, eBPF verifier bugs, Netfilter.
+Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t>F-7.2.08.
+The adversary may leverage the access from a container to the other cloud resources. The adversary can access the service principal file(used to create and manage resources), steal its credentials, and utilize them to modify or view cloud resources. 
+Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
+  </si>
+  <si>
+    <t>F-6.2.16.
+The adversary may try to access host filesystem by performing a host mounts from inside of the cluster.
+Source: Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t>F-6.2.15.
+The adversary may try to compromise Kubernetes operator by exploiting a RBAC.
+Source: Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t>F-4.2.10.
+The adversary may connect from the proxy server to cover source IP, external to cluster, and avoid the detection mechanisms. 
+Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t>F-4.2.11.
+The adversary may utilize a dynamic domain name resolution to perform a DNS tunneling or exfiltration.
+Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t>F-4.2.12.
+The adversary may try to exploit a shadow Admission control or API server.  They may establish a privileged RBAC to get a reverse shell or exploit vulnerable kube-apiserver versions to change the admission controller validation rules. For example, changing the changeAllowed label to true allows bypassing the admission controller validation rules, permitting any changes on the cluster nodes without validation. 
+Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t>F-7.2.10.
+The adversary may try to compromize Kubernetes operator by exploiting a RBAC lateral jumps.
+Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t>F-9.1.04.
+The adversary may collect internal data using automatic data gathering techniques. The adversary may use cloud APIs, command-line interfaces, or transform services to collect information in the cloud environments automatically.
+Source: https://attack.mitre.org/techniques/T1119/</t>
+  </si>
+  <si>
+    <t>F-11.2.06.
+The adversary may try to perform a personally identifiable information (PII) or IP exfiltration on the cluster or cloud datastores, and local accounts.
+Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t>F-1.0.02.
+The adversary may access the system via external remote services (e.g., VPNs), which allow them to connect from the remote location to the system. In the case of containerized environments, there are sensitive interfaces that are not meant to be exposed publicly. But sometimes due to misconfigured environments, they can be exposed. As they don't require authentication adversaries can use them to deploy a container or run malicious code. Examples of those interfaces are Docker API, Kubernetes API server, kublet, Kubeflow. 
+Source: https://attack.mitre.org/techniques/T1133/ https://www.microsoft.com/security/blog/2021/03/23/secure-containerized-environments-with-updated-threat-matrix-for-kubernetes/</t>
+  </si>
+  <si>
+    <t>F-1.1.04.
+The adversary may try to compromise an application or devise facing the internet to bring unexpected behavior. In cloud based or containerized environments, it can cause taking advantage of the underlying infrastructure. This makes it possible for adversaries to access container API or container host.  
+Source: https://attack.mitre.org/techniques/T1190/</t>
+  </si>
+  <si>
+    <t>F-1.2.08.
+The adversary may compromise a host utilizing credentials leak, stuffing, or by performing a supply chain compromise, thus using the least secured link in the system, for example unpatched services.
+Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F-2.0.01.
+The adversary may publish a malicious image in the public repository. Adversaries may try to hide the fact that the image is malicious by matching a legitimate name. Thus, users might use the image without realizing that it is malicious. This leads to the execution of code that can be used for starting cryptocurrency mining on the instance or container. 
+Source: https://attack.mitre.org/techniques/T1204/003/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F-2.2.02. 
+The adversary may compromise the container administration services such as kublet, the Kubernetes API server, and the Docker daemon. This can allow them to remotely manage containers in the environment and execute commands. For example, in Docker, the docker exec can be used to execute commands in the running container. In the Kubernetes, execution of commands can be gained by using kubectl exec, the kublet, the Kubernetes API server, and having a proper access level.
+Source: https://attack.mitre.org/techniques/T1609/ </t>
+  </si>
+  <si>
+    <t>F-2.2.05.
+The adversary may compromise the running SSH server inside of a container. Having legitimate credentials gained by phishing or brute-forcing, an adversary may remotely access a container. 
+Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F-2.2.06.
+The adversary may inject a sidecar container in the legitimate pod of the cluster to avoid adding a new pod. In Kubernete, pod is one or a group of containers in the shared network. A sidecar container is a container that exists next to the main containers in the pod. 
+Source: https://www.microsoft.com/security/blog/2021/03/23/secure-containerized-environments-with-updated-threat-matrix-for-kubernetes/ </t>
+  </si>
+  <si>
+    <t>F-2.2.07.
+The adversary may try to get remote code execution in the application. Utilizing a remote code execution, an adversary can directly take over the container on the system and deploy a malware.
+Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F-2.3.12.
+The adversary may exploit the weakest/less secure link in the CI/CD pipeline. Mainly targeted areas are exploits on widely used open-source packages, open-source vulnerabilities, compromised CI/CD tools, and changes in the build process.  
+Source: https://blog.aquasec.com/software-supply-chain-attacks-2021
+</t>
+  </si>
+  <si>
+    <t>F-4.4.15.
+The adversary may use compromised credentials of existing accounts. Obtained certificates can be used to get increased privileges in the system and provide access to restricted network areas. 
+Different types of accounts and credentials can be targeted, for example, cloud credentials, default accounts, local accounts.
+Source: https://attack.mitre.org/techniques/T1078/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F-4.2.04.
+The adversary may compromise job scheduling in containerized environments. It can be used to schedule the deployment of a container that executes malicious code. Container job scheduling works similarly to the Cron job in Linux, thus performing defined tasks in a designated time. 
+CronJob in Kubernetes can be used to schedule a specific Job. For example, a Job that executes a malicious code in the Pod of a cluster.  
+Source: https://attack.mitre.org/techniques/T1053/007/ </t>
+  </si>
+  <si>
+    <t>F-3.2.09.
+The adversary may try to perform a Node to cluster escalation. They may utilize stolen credentials to get cluster access or perform a node label rebinding attack.
+Source: Hacking Kubernetes
+By Andrew Martin, Michael Hausenblas.  https://learning.oreilly.com/library/view/hacking-kubernetes/9781492081722/</t>
+  </si>
+  <si>
+    <t>F-3.2.07.
+The adversary may leverage the access from a container to the other cloud resources. The adversary can try to access the service principal file(used to create and manage resources), steal its credentials, and utilize them to modify or view cloud resources. 
+Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
+  </si>
+  <si>
+    <t>F-8.0.01.
+The adversary may use alternate authentication material to access the target system. For example, web session cookies are commonly used in cloud web applications. Session cookie keeps the user logged in to the application, even when application is not actively used. Thus, the adversary may try to steal a cookie to bypass the log in and access the data available to the victim use. In containerized environments, secrets, including application credentials, can be stored in the configuration files and adversaries may attempt to retrieve the secrets to escalate privileges.
+Source: https://attack.mitre.org/techniques/T1550/ https://attack.mitre.org/techniques/T1550/004/ https://attack.mitre.org/techniques/T1550/001/ https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
+  </si>
+  <si>
+    <t>F-7.2.09.
+The adversary may attack other containers in the cluster utilizing allowed network traffic between pods. To perform this technique, an adversary have to have access to at least one container in the cluster.
+Source: https://www.microsoft.com/security/blog/2020/04/02/attack-matrix-kubernetes/</t>
+  </si>
+  <si>
+    <t>F-9.1.03.
+The adversary may stage data in a staging area (specific location in the system)  before exfiltrating it. The adversary can stage data to a particular instance or a virtual machine in cloud environments. 
+Source: https://attack.mitre.org/techniques/T1074/</t>
+  </si>
+  <si>
+    <t>F-10.1.01.
+The adversary may exfiltrate data and backups from one cloud account to another within the same cloud provider to avoid detection. This transfer within the same cloud provider might be more difficult to be monitored, unlike data transfers over external network interfaces.
+Source: https://attack.mitre.org/techniques/T1537/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -3377,18 +1214,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -3519,43 +1344,79 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3563,67 +1424,43 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3633,6 +1470,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3963,21 +1809,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BBF58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="88" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="G13" zoomScale="113" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.1640625" style="23" customWidth="1"/>
-    <col min="2" max="2" width="35.33203125" style="23" customWidth="1"/>
-    <col min="3" max="3" width="50.83203125" style="23" customWidth="1"/>
-    <col min="4" max="4" width="39" style="23" customWidth="1"/>
-    <col min="5" max="5" width="44.5" style="23" customWidth="1"/>
-    <col min="6" max="6" width="51" style="23" customWidth="1"/>
+    <col min="1" max="1" width="65.33203125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="50.83203125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="63.33203125" style="23" customWidth="1"/>
+    <col min="4" max="4" width="50.33203125" style="23" customWidth="1"/>
+    <col min="5" max="5" width="48.5" style="23" customWidth="1"/>
+    <col min="6" max="6" width="57.83203125" style="23" customWidth="1"/>
     <col min="7" max="7" width="46" style="23" customWidth="1"/>
     <col min="8" max="8" width="50.5" style="23" customWidth="1"/>
     <col min="9" max="9" width="34.5" style="23" customWidth="1"/>
@@ -5422,28 +3268,28 @@
     </row>
     <row r="2" spans="1:1410" s="22" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>192</v>
+        <v>154</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>15</v>
@@ -6854,39 +4700,39 @@
       <c r="BBE2" s="21"/>
       <c r="BBF2" s="21"/>
     </row>
-    <row r="3" spans="1:1410" s="22" customFormat="1" ht="294" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1410" s="22" customFormat="1" ht="337" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>65</v>
+        <v>188</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>239</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="D3" s="39" t="s">
-        <v>253</v>
+        <v>190</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>245</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>254</v>
+        <v>189</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>167</v>
+        <v>133</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>174</v>
+        <v>201</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>202</v>
+        <v>249</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>226</v>
+        <v>204</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>227</v>
+        <v>187</v>
       </c>
       <c r="L3" s="21"/>
       <c r="M3" s="21"/>
@@ -8292,7 +6138,7 @@
       <c r="A4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="32" t="s">
         <v>44</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -8302,7 +6148,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>12</v>
@@ -8314,13 +6160,13 @@
         <v>14</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="L4" s="21"/>
       <c r="M4" s="21"/>
@@ -9724,37 +7570,37 @@
     </row>
     <row r="5" spans="1:1410" s="22" customFormat="1" ht="388" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>190</v>
+        <v>236</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>240</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>99</v>
+        <v>198</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>168</v>
+        <v>200</v>
       </c>
       <c r="G5" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>223</v>
-      </c>
       <c r="K5" s="8" t="s">
-        <v>228</v>
+        <v>206</v>
       </c>
       <c r="L5" s="21"/>
       <c r="M5" s="21"/>
@@ -11158,18 +9004,18 @@
     </row>
     <row r="6" spans="1:1410" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>46</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="42" t="s">
         <v>29</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -11182,7 +9028,7 @@
         <v>22</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="J6" s="14" t="s">
         <v>54</v>
@@ -11192,38 +9038,38 @@
       </c>
     </row>
     <row r="7" spans="1:1410" s="21" customFormat="1" ht="263" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>68</v>
+      <c r="A7" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>193</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>69</v>
+        <v>195</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="F7" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="J7" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="H7" s="4" t="s">
+      <c r="K7" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="J7" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:1410" s="21" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -11231,28 +9077,28 @@
         <v>18</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>31</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="G8" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="12" t="s">
-        <v>62</v>
+      <c r="I8" s="31" t="s">
+        <v>158</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>55</v>
@@ -11261,39 +9107,39 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:1410" s="21" customFormat="1" ht="306" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1410" s="21" customFormat="1" ht="255" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>72</v>
+        <v>237</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>194</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>74</v>
+        <v>246</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>145</v>
+        <v>118</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="G9" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="H9" s="40" t="s">
+        <v>203</v>
+      </c>
+      <c r="I9" s="45" t="s">
+        <v>234</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="K9" s="4" t="s">
         <v>178</v>
-      </c>
-      <c r="H9" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="I9" s="36" t="s">
-        <v>155</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:1410" ht="98" customHeight="1" x14ac:dyDescent="0.2">
@@ -11301,79 +9147,75 @@
         <v>45</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>26</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="H10" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="32" t="s">
-        <v>196</v>
-      </c>
+      <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:1410" ht="275" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>76</v>
+      <c r="A11" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="B11" s="44" t="s">
+        <v>241</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>78</v>
+        <v>209</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>201</v>
+        <v>162</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="H11" s="35" t="s">
-        <v>209</v>
-      </c>
-      <c r="I11" s="38" t="s">
-        <v>221</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="H11" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="4" t="s">
-        <v>231</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:1410" ht="79" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>47</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D12" s="36" t="s">
-        <v>216</v>
+        <v>82</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>172</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>48</v>
@@ -11384,281 +9226,281 @@
       <c r="G12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="35" t="s">
+      <c r="H12" s="33" t="s">
         <v>59</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="1"/>
       <c r="K12" s="12" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:1410" ht="309" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>80</v>
+      <c r="A13" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>242</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>81</v>
+        <v>86</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>210</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>212</v>
+        <v>171</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="H13" s="35" t="s">
-        <v>210</v>
+        <v>143</v>
+      </c>
+      <c r="H13" s="33" t="s">
+        <v>169</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="36" t="s">
-        <v>252</v>
+      <c r="K13" s="44" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:1410" ht="80" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="B14" s="12" t="s">
+      <c r="A14" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="40" t="s">
         <v>56</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>148</v>
+        <v>121</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>165</v>
+        <v>131</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>30</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="I14" s="2"/>
+        <v>91</v>
+      </c>
       <c r="J14" s="1"/>
       <c r="K14" s="13" t="s">
-        <v>195</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:1410" ht="371" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="36" t="s">
-        <v>234</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>156</v>
+      <c r="A15" s="40" t="s">
+        <v>207</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>243</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>93</v>
+        <v>196</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>213</v>
+        <v>248</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="H15" s="35" t="s">
-        <v>211</v>
-      </c>
-      <c r="I15" s="2"/>
+        <v>144</v>
+      </c>
+      <c r="H15" s="33" t="s">
+        <v>170</v>
+      </c>
       <c r="J15" s="1"/>
-      <c r="K15" s="38" t="s">
-        <v>232</v>
+      <c r="K15" s="36" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:1410" ht="151" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>49</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>172</v>
+        <v>137</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>40</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>114</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:9" ht="397" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="36" t="s">
-        <v>235</v>
-      </c>
-      <c r="B17" s="36" t="s">
-        <v>236</v>
+      <c r="A17" s="44" t="s">
+        <v>238</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>214</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="D17" s="36" t="s">
-        <v>243</v>
+        <v>208</v>
+      </c>
+      <c r="D17" s="44" t="s">
+        <v>222</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="F17" s="29" t="s">
-        <v>173</v>
+        <v>199</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>138</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="H17" s="35" t="s">
-        <v>214</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="H17" s="44" t="s">
+        <v>227</v>
+      </c>
+      <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:9" ht="97" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>34</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>193</v>
+        <v>155</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="36" t="s">
-        <v>120</v>
+      <c r="H18" s="34" t="s">
+        <v>96</v>
       </c>
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" ht="291" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="36" t="s">
-        <v>233</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C19" s="36" t="s">
-        <v>241</v>
-      </c>
-      <c r="D19" s="36" t="s">
-        <v>244</v>
+      <c r="A19" s="40" t="s">
+        <v>211</v>
+      </c>
+      <c r="B19" s="41" t="s">
+        <v>182</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="D19" s="44" t="s">
+        <v>247</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>200</v>
+        <v>161</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="H19" s="36" t="s">
-        <v>217</v>
+        <v>146</v>
+      </c>
+      <c r="H19" s="44" t="s">
+        <v>250</v>
       </c>
       <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:9" ht="115" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
-        <v>125</v>
+      <c r="A20" s="40" t="s">
+        <v>212</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>128</v>
+        <v>102</v>
+      </c>
+      <c r="D20" s="44" t="s">
+        <v>103</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="H20" s="35" t="s">
-        <v>204</v>
+        <v>105</v>
+      </c>
+      <c r="H20" s="44" t="s">
+        <v>164</v>
       </c>
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" ht="234" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="36" t="s">
-        <v>237</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21" s="36" t="s">
-        <v>215</v>
-      </c>
-      <c r="D21" s="36" t="s">
-        <v>245</v>
-      </c>
-      <c r="E21" s="36" t="s">
-        <v>249</v>
+      <c r="A21" s="40" t="s">
+        <v>213</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="C21" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="D21" s="44" t="s">
+        <v>223</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>230</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>199</v>
+        <v>160</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="H21" s="35" t="s">
-        <v>154</v>
+        <v>147</v>
+      </c>
+      <c r="H21" s="44" t="s">
+        <v>233</v>
       </c>
       <c r="I21" s="2"/>
     </row>
     <row r="22" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="21"/>
       <c r="B22" s="14" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="4" t="s">
@@ -11667,30 +9509,28 @@
       <c r="H22" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="I22" s="2"/>
     </row>
     <row r="23" spans="1:9" ht="221" x14ac:dyDescent="0.2">
       <c r="A23" s="21"/>
-      <c r="B23" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C23" s="36" t="s">
-        <v>238</v>
-      </c>
-      <c r="D23" s="36" t="s">
-        <v>246</v>
-      </c>
-      <c r="E23" s="36" t="s">
-        <v>250</v>
+      <c r="B23" s="38" t="s">
+        <v>184</v>
+      </c>
+      <c r="C23" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="D23" s="44" t="s">
+        <v>224</v>
+      </c>
+      <c r="E23" s="44" t="s">
+        <v>231</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="H23" s="37" t="s">
-        <v>218</v>
-      </c>
-      <c r="I23" s="2"/>
+        <v>148</v>
+      </c>
+      <c r="H23" s="35" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="24" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="14" t="s">
@@ -11700,7 +9540,7 @@
         <v>57</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>57</v>
@@ -11712,44 +9552,46 @@
       <c r="H24" s="14" t="s">
         <v>53</v>
       </c>
+      <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" ht="297" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="C25" s="36" t="s">
-        <v>239</v>
-      </c>
-      <c r="D25" s="36" t="s">
-        <v>247</v>
-      </c>
-      <c r="E25" s="36" t="s">
-        <v>251</v>
+      <c r="B25" s="43" t="s">
+        <v>244</v>
+      </c>
+      <c r="C25" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="D25" s="44" t="s">
+        <v>225</v>
+      </c>
+      <c r="E25" s="44" t="s">
+        <v>232</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="H25" s="37" t="s">
-        <v>207</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="H25" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B26" s="14" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>50</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="6" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
       <c r="H26" s="23" t="s">
         <v>36</v>
@@ -11757,27 +9599,27 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" ht="289" x14ac:dyDescent="0.2">
-      <c r="B27" s="14" t="s">
-        <v>88</v>
+      <c r="B27" s="38" t="s">
+        <v>185</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="D27" s="36" t="s">
-        <v>248</v>
+        <v>221</v>
+      </c>
+      <c r="D27" s="44" t="s">
+        <v>226</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="6" t="s">
-        <v>187</v>
+        <v>150</v>
       </c>
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="B28" s="14" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>50</v>
@@ -11786,11 +9628,11 @@
         <v>51</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="F28" s="1"/>
-      <c r="G28" s="35" t="s">
-        <v>189</v>
+      <c r="G28" s="33" t="s">
+        <v>152</v>
       </c>
       <c r="H28" s="23" t="s">
         <v>36</v>
@@ -11798,21 +9640,21 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" ht="323" x14ac:dyDescent="0.2">
-      <c r="B29" s="14" t="s">
-        <v>86</v>
+      <c r="B29" s="38" t="s">
+        <v>186</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" s="37" t="s">
-        <v>146</v>
+        <v>70</v>
+      </c>
+      <c r="D29" s="35" t="s">
+        <v>119</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>162</v>
+        <v>128</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="27" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="I29" s="1"/>
     </row>
@@ -11824,33 +9666,33 @@
         <v>36</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="F30" s="1"/>
-      <c r="G30" s="35" t="s">
-        <v>208</v>
+      <c r="G30" s="33" t="s">
+        <v>167</v>
       </c>
       <c r="H30" s="23" t="s">
         <v>36</v>
       </c>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" ht="119" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C31" s="14" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>163</v>
+        <v>129</v>
       </c>
       <c r="F31" s="1"/>
-      <c r="G31" s="12" t="s">
-        <v>153</v>
+      <c r="G31" s="44" t="s">
+        <v>229</v>
       </c>
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="C32" s="14" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="D32" s="23" t="s">
         <v>36</v>
@@ -11862,43 +9704,41 @@
         <v>36</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>160</v>
+        <v>126</v>
       </c>
       <c r="H32" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" ht="153" x14ac:dyDescent="0.2">
-      <c r="C33" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="E33" s="33" t="s">
+    <row r="33" spans="1:9" ht="170" x14ac:dyDescent="0.2">
+      <c r="C33" s="41" t="s">
         <v>197</v>
       </c>
-      <c r="G33" s="28" t="s">
-        <v>152</v>
+      <c r="E33" s="43" t="s">
+        <v>216</v>
+      </c>
+      <c r="G33" s="44" t="s">
+        <v>228</v>
       </c>
       <c r="H33" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="C34" s="14" t="s">
-        <v>159</v>
+    <row r="34" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="C34" s="41" t="s">
+        <v>215</v>
       </c>
       <c r="D34" s="23" t="s">
         <v>36</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="F34" s="23" t="s">
         <v>36</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="H34" s="23" t="s">
         <v>36</v>
@@ -11906,18 +9746,21 @@
     </row>
     <row r="35" spans="1:9" ht="321" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C35" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="E35" s="29" t="s">
-        <v>164</v>
-      </c>
-      <c r="F35" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="F35" s="29" t="s">
         <v>36</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>198</v>
+        <v>159</v>
       </c>
       <c r="H35" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="I35" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -11928,11 +9771,14 @@
       <c r="D36" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="31"/>
+      <c r="E36" s="30"/>
       <c r="F36" s="23" t="s">
         <v>36</v>
       </c>
       <c r="H36" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="I36" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -11945,7 +9791,7 @@
       <c r="D37" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="E37" s="31"/>
+      <c r="E37" s="30"/>
       <c r="F37" s="23" t="s">
         <v>36</v>
       </c>
@@ -11965,7 +9811,7 @@
       <c r="D38" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="E38" s="31"/>
+      <c r="E38" s="30"/>
       <c r="F38" s="23" t="s">
         <v>36</v>
       </c>
@@ -11986,7 +9832,7 @@
       <c r="D39" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="31"/>
+      <c r="E39" s="30"/>
       <c r="F39" s="23" t="s">
         <v>36</v>
       </c>
@@ -12319,9 +10165,6 @@
       <c r="F56" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="I56" s="23" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="57" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" s="23" t="s">
@@ -12331,9 +10174,6 @@
         <v>36</v>
       </c>
       <c r="F57" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="I57" s="23" t="s">
         <v>36</v>
       </c>
     </row>
@@ -12345,7 +10185,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -12482,18 +10321,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12515,14 +10354,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0702E8AA-3C34-4832-A076-EFC50130F7BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F45A948D-B766-4C4F-A553-1496C93F67CB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -12536,4 +10367,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0702E8AA-3C34-4832-A076-EFC50130F7BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>